<commit_message>
dinamic date on pdf
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="617">
   <si>
     <t>S051</t>
   </si>
@@ -1600,6 +1600,282 @@
   </si>
   <si>
     <t>static/uploads/S096.png</t>
+  </si>
+  <si>
+    <t>S097</t>
+  </si>
+  <si>
+    <t>3309120108049001</t>
+  </si>
+  <si>
+    <t>ALE SANDRO DWI SAPUTRA</t>
+  </si>
+  <si>
+    <t>0895340453050</t>
+  </si>
+  <si>
+    <t>KLIWONAN RT 02/07 DESA JERON, KEC NOGOSARI, KAB BOYOLALI</t>
+  </si>
+  <si>
+    <t>static/uploads/S097.png</t>
+  </si>
+  <si>
+    <t>S098</t>
+  </si>
+  <si>
+    <t>3314011507800004</t>
+  </si>
+  <si>
+    <t>LASNO</t>
+  </si>
+  <si>
+    <t>082220833940</t>
+  </si>
+  <si>
+    <t>KEDEN WETAN RT 14 DESA KEDEN, KEC KALIJAMBE, KAB SRAGEN</t>
+  </si>
+  <si>
+    <t>static/uploads/S098.png</t>
+  </si>
+  <si>
+    <t>S099</t>
+  </si>
+  <si>
+    <t>3319060511840002</t>
+  </si>
+  <si>
+    <t>MATTORI</t>
+  </si>
+  <si>
+    <t>082322083412</t>
+  </si>
+  <si>
+    <t>RT 01/07 DESA TERBAN, KEC JEKULO, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S099.png</t>
+  </si>
+  <si>
+    <t>S100</t>
+  </si>
+  <si>
+    <t>3319080808890003</t>
+  </si>
+  <si>
+    <t>AZWAR ANAS</t>
+  </si>
+  <si>
+    <t>085225324480</t>
+  </si>
+  <si>
+    <t>NGARINGAN RT 06/06 DESA KLUMPIT, KEC GEBOG, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S100.png</t>
+  </si>
+  <si>
+    <t>S101</t>
+  </si>
+  <si>
+    <t>3318081006740001</t>
+  </si>
+  <si>
+    <t>WAWAN SAFUAN</t>
+  </si>
+  <si>
+    <t>085281656966</t>
+  </si>
+  <si>
+    <t>LANGGEN RT 01/03 DESA LANGGENHARJO, KEC JUWANA, KAB PATI</t>
+  </si>
+  <si>
+    <t>static/uploads/S101.png</t>
+  </si>
+  <si>
+    <t>S102</t>
+  </si>
+  <si>
+    <t>3319062305970004</t>
+  </si>
+  <si>
+    <t>NURUL FARIHIN</t>
+  </si>
+  <si>
+    <t>082325160701</t>
+  </si>
+  <si>
+    <t>RT 05/07 DESA BULUNG KULON, KEC JEKULO, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S102.png</t>
+  </si>
+  <si>
+    <t>S103</t>
+  </si>
+  <si>
+    <t>3173061807990008</t>
+  </si>
+  <si>
+    <t>HARYONO</t>
+  </si>
+  <si>
+    <t>RT 04/01 DESA PADANG JAYA, KEC MAJENANG, KAB CILACAP</t>
+  </si>
+  <si>
+    <t>static/uploads/S103.png</t>
+  </si>
+  <si>
+    <t>S104</t>
+  </si>
+  <si>
+    <t>33181219068200011</t>
+  </si>
+  <si>
+    <t>KIYANTO</t>
+  </si>
+  <si>
+    <t>085327340315</t>
+  </si>
+  <si>
+    <t>MAWAR RT 02/05 DESA JAMBEAN KIDUL, KEC MARGOREJO, KAB PATI</t>
+  </si>
+  <si>
+    <t>static/uploads/S104.png</t>
+  </si>
+  <si>
+    <t>S105</t>
+  </si>
+  <si>
+    <t>3318042004630001</t>
+  </si>
+  <si>
+    <t>TRIYONO</t>
+  </si>
+  <si>
+    <t>082146354406</t>
+  </si>
+  <si>
+    <t>BLLIBAK RT 02/02 DESA PULOREJO, KEC WINONG, KAB PATI</t>
+  </si>
+  <si>
+    <t>static/uploads/S105.png</t>
+  </si>
+  <si>
+    <t>S106</t>
+  </si>
+  <si>
+    <t>ACHMAD SYAFI'I</t>
+  </si>
+  <si>
+    <t>static/uploads/S106.png</t>
+  </si>
+  <si>
+    <t>S107</t>
+  </si>
+  <si>
+    <t>33190823027700001</t>
+  </si>
+  <si>
+    <t>MOCH RIDWAN</t>
+  </si>
+  <si>
+    <t>081325416658</t>
+  </si>
+  <si>
+    <t>RT 02/01 DESAA KARANGMALANG, KEC GEBOG, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S107.png</t>
+  </si>
+  <si>
+    <t>S108</t>
+  </si>
+  <si>
+    <t>3319060305720002</t>
+  </si>
+  <si>
+    <t>SURYANI</t>
+  </si>
+  <si>
+    <t>081391387397</t>
+  </si>
+  <si>
+    <t>RT 02/07 DESA TERBAN, KEC JEKULO, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S108.png</t>
+  </si>
+  <si>
+    <t>S109</t>
+  </si>
+  <si>
+    <t>3319062710840005</t>
+  </si>
+  <si>
+    <t>JOKO SAPUTRO</t>
+  </si>
+  <si>
+    <t>081228768461</t>
+  </si>
+  <si>
+    <t>RT 04/03 DESA SIDOMULYO, KEC JEKULO, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S109.png</t>
+  </si>
+  <si>
+    <t>S110</t>
+  </si>
+  <si>
+    <t>3319032205790001</t>
+  </si>
+  <si>
+    <t>ABDUL MALIK</t>
+  </si>
+  <si>
+    <t>082227937092</t>
+  </si>
+  <si>
+    <t>RT 03/06 DESA LORAM WETAN, KEC JATI, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S110.png</t>
+  </si>
+  <si>
+    <t>S111</t>
+  </si>
+  <si>
+    <t>3319033012640001</t>
+  </si>
+  <si>
+    <t>ABU BADARI</t>
+  </si>
+  <si>
+    <t>085290148365</t>
+  </si>
+  <si>
+    <t>RT 02/04 DESA JATI KULON, KEC JATI, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S111.png</t>
+  </si>
+  <si>
+    <t>S112</t>
+  </si>
+  <si>
+    <t>3319020211010004</t>
+  </si>
+  <si>
+    <t>MUUHAMMAD NI'MAL MAULANA SISWANTO</t>
+  </si>
+  <si>
+    <t>085523784468</t>
+  </si>
+  <si>
+    <t>RT 04/02 DESA KALIPUTU, KEC KOTA, KAB KUDUS</t>
+  </si>
+  <si>
+    <t>static/uploads/S112.png</t>
   </si>
 </sst>
 </file>
@@ -4796,6 +5072,470 @@
         <v>524</v>
       </c>
     </row>
+    <row r="101">
+      <c r="A101" t="s">
+        <v>525</v>
+      </c>
+      <c r="B101" t="s">
+        <v>1</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="D101" t="s">
+        <v>527</v>
+      </c>
+      <c r="E101" t="s">
+        <v>528</v>
+      </c>
+      <c r="F101" t="s">
+        <v>529</v>
+      </c>
+      <c r="G101">
+        <v>0</v>
+      </c>
+      <c r="H101" t="s">
+        <v>2</v>
+      </c>
+      <c r="I101" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="s">
+        <v>531</v>
+      </c>
+      <c r="B102" t="s">
+        <v>1</v>
+      </c>
+      <c r="C102" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="D102" t="s">
+        <v>533</v>
+      </c>
+      <c r="E102" t="s">
+        <v>534</v>
+      </c>
+      <c r="F102" t="s">
+        <v>535</v>
+      </c>
+      <c r="G102">
+        <v>0</v>
+      </c>
+      <c r="H102" t="s">
+        <v>2</v>
+      </c>
+      <c r="I102" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="s">
+        <v>537</v>
+      </c>
+      <c r="B103" t="s">
+        <v>1</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="D103" t="s">
+        <v>539</v>
+      </c>
+      <c r="E103" t="s">
+        <v>540</v>
+      </c>
+      <c r="F103" t="s">
+        <v>541</v>
+      </c>
+      <c r="G103">
+        <v>0</v>
+      </c>
+      <c r="H103" t="s">
+        <v>2</v>
+      </c>
+      <c r="I103" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="s">
+        <v>543</v>
+      </c>
+      <c r="B104" t="s">
+        <v>1</v>
+      </c>
+      <c r="C104" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="D104" t="s">
+        <v>545</v>
+      </c>
+      <c r="E104" t="s">
+        <v>546</v>
+      </c>
+      <c r="F104" t="s">
+        <v>547</v>
+      </c>
+      <c r="G104">
+        <v>0</v>
+      </c>
+      <c r="H104" t="s">
+        <v>2</v>
+      </c>
+      <c r="I104" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="s">
+        <v>549</v>
+      </c>
+      <c r="B105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="D105" t="s">
+        <v>551</v>
+      </c>
+      <c r="E105" t="s">
+        <v>552</v>
+      </c>
+      <c r="F105" t="s">
+        <v>553</v>
+      </c>
+      <c r="G105">
+        <v>0</v>
+      </c>
+      <c r="H105" t="s">
+        <v>2</v>
+      </c>
+      <c r="I105" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="s">
+        <v>555</v>
+      </c>
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="C106" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="D106" t="s">
+        <v>557</v>
+      </c>
+      <c r="E106" t="s">
+        <v>558</v>
+      </c>
+      <c r="F106" t="s">
+        <v>559</v>
+      </c>
+      <c r="G106">
+        <v>0</v>
+      </c>
+      <c r="H106" t="s">
+        <v>2</v>
+      </c>
+      <c r="I106" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="s">
+        <v>561</v>
+      </c>
+      <c r="B107" t="s">
+        <v>1</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>562</v>
+      </c>
+      <c r="D107" t="s">
+        <v>563</v>
+      </c>
+      <c r="E107" t="s">
+        <v>175</v>
+      </c>
+      <c r="F107" t="s">
+        <v>564</v>
+      </c>
+      <c r="G107">
+        <v>0</v>
+      </c>
+      <c r="H107" t="s">
+        <v>2</v>
+      </c>
+      <c r="I107" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="s">
+        <v>566</v>
+      </c>
+      <c r="B108" t="s">
+        <v>1</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>567</v>
+      </c>
+      <c r="D108" t="s">
+        <v>568</v>
+      </c>
+      <c r="E108" t="s">
+        <v>569</v>
+      </c>
+      <c r="F108" t="s">
+        <v>570</v>
+      </c>
+      <c r="G108">
+        <v>0</v>
+      </c>
+      <c r="H108" t="s">
+        <v>2</v>
+      </c>
+      <c r="I108" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="s">
+        <v>572</v>
+      </c>
+      <c r="B109" t="s">
+        <v>1</v>
+      </c>
+      <c r="C109" s="9" t="s">
+        <v>573</v>
+      </c>
+      <c r="D109" t="s">
+        <v>574</v>
+      </c>
+      <c r="E109" t="s">
+        <v>575</v>
+      </c>
+      <c r="F109" t="s">
+        <v>576</v>
+      </c>
+      <c r="G109">
+        <v>0</v>
+      </c>
+      <c r="H109" t="s">
+        <v>2</v>
+      </c>
+      <c r="I109" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="s">
+        <v>578</v>
+      </c>
+      <c r="B110" t="s">
+        <v>1</v>
+      </c>
+      <c r="C110" s="9" t="s">
+        <v>292</v>
+      </c>
+      <c r="D110" t="s">
+        <v>579</v>
+      </c>
+      <c r="E110" t="s">
+        <v>175</v>
+      </c>
+      <c r="F110" t="s">
+        <v>294</v>
+      </c>
+      <c r="G110">
+        <v>0</v>
+      </c>
+      <c r="H110" t="s">
+        <v>2</v>
+      </c>
+      <c r="I110" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="s">
+        <v>581</v>
+      </c>
+      <c r="B111" t="s">
+        <v>1</v>
+      </c>
+      <c r="C111" s="9" t="s">
+        <v>582</v>
+      </c>
+      <c r="D111" t="s">
+        <v>583</v>
+      </c>
+      <c r="E111" t="s">
+        <v>584</v>
+      </c>
+      <c r="F111" t="s">
+        <v>585</v>
+      </c>
+      <c r="G111">
+        <v>0</v>
+      </c>
+      <c r="H111" t="s">
+        <v>2</v>
+      </c>
+      <c r="I111" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="s">
+        <v>587</v>
+      </c>
+      <c r="B112" t="s">
+        <v>1</v>
+      </c>
+      <c r="C112" s="9" t="s">
+        <v>588</v>
+      </c>
+      <c r="D112" t="s">
+        <v>589</v>
+      </c>
+      <c r="E112" t="s">
+        <v>590</v>
+      </c>
+      <c r="F112" t="s">
+        <v>591</v>
+      </c>
+      <c r="G112">
+        <v>0</v>
+      </c>
+      <c r="H112" t="s">
+        <v>2</v>
+      </c>
+      <c r="I112" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="s">
+        <v>593</v>
+      </c>
+      <c r="B113" t="s">
+        <v>1</v>
+      </c>
+      <c r="C113" s="9" t="s">
+        <v>594</v>
+      </c>
+      <c r="D113" t="s">
+        <v>595</v>
+      </c>
+      <c r="E113" t="s">
+        <v>596</v>
+      </c>
+      <c r="F113" t="s">
+        <v>597</v>
+      </c>
+      <c r="G113">
+        <v>0</v>
+      </c>
+      <c r="H113" t="s">
+        <v>2</v>
+      </c>
+      <c r="I113" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="s">
+        <v>599</v>
+      </c>
+      <c r="B114" t="s">
+        <v>1</v>
+      </c>
+      <c r="C114" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="D114" t="s">
+        <v>601</v>
+      </c>
+      <c r="E114" t="s">
+        <v>602</v>
+      </c>
+      <c r="F114" t="s">
+        <v>603</v>
+      </c>
+      <c r="G114">
+        <v>0</v>
+      </c>
+      <c r="H114" t="s">
+        <v>2</v>
+      </c>
+      <c r="I114" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="s">
+        <v>605</v>
+      </c>
+      <c r="B115" t="s">
+        <v>1</v>
+      </c>
+      <c r="C115" s="9" t="s">
+        <v>606</v>
+      </c>
+      <c r="D115" t="s">
+        <v>607</v>
+      </c>
+      <c r="E115" t="s">
+        <v>608</v>
+      </c>
+      <c r="F115" t="s">
+        <v>609</v>
+      </c>
+      <c r="G115">
+        <v>0</v>
+      </c>
+      <c r="H115" t="s">
+        <v>2</v>
+      </c>
+      <c r="I115" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="s">
+        <v>611</v>
+      </c>
+      <c r="B116" t="s">
+        <v>1</v>
+      </c>
+      <c r="C116" s="9" t="s">
+        <v>612</v>
+      </c>
+      <c r="D116" t="s">
+        <v>613</v>
+      </c>
+      <c r="E116" t="s">
+        <v>614</v>
+      </c>
+      <c r="F116" t="s">
+        <v>615</v>
+      </c>
+      <c r="G116">
+        <v>0</v>
+      </c>
+      <c r="H116" t="s">
+        <v>2</v>
+      </c>
+      <c r="I116" t="s">
+        <v>616</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>